<commit_message>
Add data provider to HotelSearchTest
</commit_message>
<xml_diff>
--- a/src/test/resources/testData.xlsx
+++ b/src/test/resources/testData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve">city</t>
   </si>
@@ -31,10 +31,13 @@
     <t xml:space="preserve">Dubai</t>
   </si>
   <si>
-    <t xml:space="preserve">xxx</t>
+    <t xml:space="preserve">Jumeirah Beach Hotel</t>
   </si>
   <si>
     <t xml:space="preserve">London</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grand Plaza Apartments</t>
   </si>
 </sst>
 </file>
@@ -112,8 +115,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -137,33 +144,33 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>3</v>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>